<commit_message>
Converted Radio IDs to indices
</commit_message>
<xml_diff>
--- a/SiK_Radios.xlsx
+++ b/SiK_Radios.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Miers\Documents\Christopher Newport University\Grad Research\Sik_Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Research\Sik_Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2253B7-3931-4784-A92D-0EE95B884F90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E00A2C9-38CD-49F6-8330-246AF239A8A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{48E60877-4D87-47E2-9DD7-EC0BD204F274}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{48E60877-4D87-47E2-9DD7-EC0BD204F274}"/>
   </bookViews>
   <sheets>
-    <sheet name="Radio IDs" sheetId="1" r:id="rId1"/>
-    <sheet name="1" sheetId="2" r:id="rId2"/>
-    <sheet name="2" sheetId="3" r:id="rId3"/>
-    <sheet name="3" sheetId="4" r:id="rId4"/>
-    <sheet name="4" sheetId="5" r:id="rId5"/>
-    <sheet name="5" sheetId="9" r:id="rId6"/>
-    <sheet name="6" sheetId="8" r:id="rId7"/>
-    <sheet name="7" sheetId="10" r:id="rId8"/>
-    <sheet name="8" sheetId="7" r:id="rId9"/>
+    <sheet name="Radio Labels" sheetId="1" r:id="rId1"/>
+    <sheet name="0" sheetId="2" r:id="rId2"/>
+    <sheet name="1" sheetId="3" r:id="rId3"/>
+    <sheet name="2" sheetId="4" r:id="rId4"/>
+    <sheet name="3" sheetId="5" r:id="rId5"/>
+    <sheet name="4" sheetId="9" r:id="rId6"/>
+    <sheet name="5" sheetId="8" r:id="rId7"/>
+    <sheet name="6" sheetId="10" r:id="rId8"/>
+    <sheet name="7" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,9 +42,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
-  <si>
-    <t>ID</t>
-  </si>
   <si>
     <t>Radio Name</t>
   </si>
@@ -127,6 +124,9 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>Label Index</t>
   </si>
 </sst>
 </file>
@@ -331,7 +331,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'1'!$A$2:$A$1000</c:f>
+              <c:f>'0'!$A$2:$A$1000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="999"/>
@@ -339,34 +339,34 @@
                   <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1.7570000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.01</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0000000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>1.8100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.02</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.7570000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.7000000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.8100000000000002E-2</c:v>
-                </c:pt>
                 <c:pt idx="9">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>5.8000000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.2000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.10299999999999999</c:v>
@@ -379,7 +379,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1'!$B$2:$B$1000</c:f>
+              <c:f>'0'!$B$2:$B$1000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="999"/>
@@ -387,34 +387,34 @@
                   <c:v>44.77</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>40.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>25.167999999999999</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>31.06</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>27.03</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35.49</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>19.809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>19.11</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>40.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>29.81</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>19.809999999999999</c:v>
-                </c:pt>
                 <c:pt idx="9">
+                  <c:v>14.94</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>10.08</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14.94</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>5.98</c:v>
@@ -874,7 +874,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'2'!$A$2:$A$1000</c:f>
+              <c:f>'1'!$A$2:$A$1000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="999"/>
@@ -910,7 +910,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'2'!$B$2:$B$1000</c:f>
+              <c:f>'1'!$B$2:$B$1000</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="999"/>
@@ -1421,7 +1421,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'3'!$A$2:$A$1001</c:f>
+              <c:f>'2'!$A$2:$A$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1000"/>
@@ -1457,7 +1457,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3'!$B$2:$B$1001</c:f>
+              <c:f>'2'!$B$2:$B$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1000"/>
@@ -1971,7 +1971,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'4'!$A$2:$A$1001</c:f>
+              <c:f>'3'!$A$2:$A$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1000"/>
@@ -2010,7 +2010,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4'!$B$2:$B$1001</c:f>
+              <c:f>'3'!$B$2:$B$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1000"/>
@@ -2527,7 +2527,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'5'!$A$2:$A$1001</c:f>
+              <c:f>'4'!$A$2:$A$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1000"/>
@@ -2566,7 +2566,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'5'!$B$2:$B$1001</c:f>
+              <c:f>'4'!$B$2:$B$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1000"/>
@@ -3083,7 +3083,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'6'!$A$2:$A$1001</c:f>
+              <c:f>'5'!$A$2:$A$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1000"/>
@@ -3122,7 +3122,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'6'!$B$2:$B$1001</c:f>
+              <c:f>'5'!$B$2:$B$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1000"/>
@@ -3639,7 +3639,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'7'!$A$2:$A$1001</c:f>
+              <c:f>'6'!$A$2:$A$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1000"/>
@@ -3678,7 +3678,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'7'!$B$2:$B$1001</c:f>
+              <c:f>'6'!$B$2:$B$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1000"/>
@@ -4195,7 +4195,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'8'!$A$2:$A$1001</c:f>
+              <c:f>'7'!$A$2:$A$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1000"/>
@@ -4234,7 +4234,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8'!$B$2:$B$1001</c:f>
+              <c:f>'7'!$B$2:$B$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1000"/>
@@ -9039,15 +9039,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>607695</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>440055</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>135255</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9674,125 +9674,126 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -9806,26 +9807,26 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1E-3</v>
       </c>
@@ -9833,87 +9834,87 @@
         <v>44.77</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>1.7570000000000001E-3</v>
+      </c>
+      <c r="B3">
+        <v>40.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="B4">
+        <v>35.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B5">
+        <v>31.06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="B6">
+        <v>29.81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="B7">
+        <v>27.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>0.01</v>
       </c>
-      <c r="B3">
+      <c r="B8">
         <v>25.167999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="B4">
-        <v>31.06</v>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="B9">
+        <v>19.809999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="B5">
-        <v>27.03</v>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.02</v>
+      </c>
+      <c r="B10">
+        <v>19.11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="B6">
-        <v>35.49</v>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="B11">
+        <v>14.94</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>0.02</v>
-      </c>
-      <c r="B7">
-        <v>19.11</v>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="B12">
+        <v>10.08</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1.7570000000000001E-3</v>
-      </c>
-      <c r="B8">
-        <v>40.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>5.7000000000000002E-3</v>
-      </c>
-      <c r="B9">
-        <v>29.81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1.8100000000000002E-2</v>
-      </c>
-      <c r="B10">
-        <v>19.809999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="B11">
-        <v>10.08</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="B12">
-        <v>14.94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.10299999999999999</v>
       </c>
@@ -9921,7 +9922,7 @@
         <v>5.98</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.193</v>
       </c>
@@ -9930,6 +9931,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B14">
+    <sortCondition descending="1" ref="B2:B14"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -9943,20 +9947,20 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.7570000000000001E-3</v>
       </c>
@@ -9964,7 +9968,7 @@
         <v>40.72</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -9972,7 +9976,7 @@
         <v>36.090000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -9980,7 +9984,7 @@
         <v>31.66</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.01</v>
       </c>
@@ -9988,7 +9992,7 @@
         <v>25.66</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.02</v>
       </c>
@@ -9996,7 +10000,7 @@
         <v>19.670000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3.2000000000000001E-2</v>
       </c>
@@ -10004,7 +10008,7 @@
         <v>15.67</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5.8000000000000003E-2</v>
       </c>
@@ -10012,7 +10016,7 @@
         <v>10.75</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.10299999999999999</v>
       </c>
@@ -10020,7 +10024,7 @@
         <v>6.49</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.2</v>
       </c>
@@ -10042,20 +10046,20 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>9.859999999999999E-4</v>
       </c>
@@ -10063,7 +10067,7 @@
         <v>39.909999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.7570000000000001E-3</v>
       </c>
@@ -10071,7 +10075,7 @@
         <v>36.56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10079,7 +10083,7 @@
         <v>31.41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10087,7 +10091,7 @@
         <v>25.06</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.01</v>
       </c>
@@ -10095,7 +10099,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.02</v>
       </c>
@@ -10103,7 +10107,7 @@
         <v>13.94</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.2000000000000001E-2</v>
       </c>
@@ -10111,7 +10115,7 @@
         <v>10.15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.8000000000000003E-2</v>
       </c>
@@ -10119,7 +10123,7 @@
         <v>5.84</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.10299999999999999</v>
       </c>
@@ -10141,20 +10145,20 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>9.859999999999999E-4</v>
       </c>
@@ -10162,7 +10166,7 @@
         <v>44.75</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.7570000000000001E-3</v>
       </c>
@@ -10170,7 +10174,7 @@
         <v>40.020000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10178,7 +10182,7 @@
         <v>35.369999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10186,7 +10190,7 @@
         <v>30.94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.01</v>
       </c>
@@ -10194,7 +10198,7 @@
         <v>24.91</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.02</v>
       </c>
@@ -10202,7 +10206,7 @@
         <v>18.940000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.2000000000000001E-2</v>
       </c>
@@ -10210,7 +10214,7 @@
         <v>14.95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.8000000000000003E-2</v>
       </c>
@@ -10218,7 +10222,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.10299999999999999</v>
       </c>
@@ -10226,7 +10230,7 @@
         <v>5.93</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.2</v>
       </c>
@@ -10248,20 +10252,20 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>9.859999999999999E-4</v>
       </c>
@@ -10269,7 +10273,7 @@
         <v>46.29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.7570000000000001E-3</v>
       </c>
@@ -10277,7 +10281,7 @@
         <v>40.659999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10285,7 +10289,7 @@
         <v>36.71</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10293,7 +10297,7 @@
         <v>32.21</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.01</v>
       </c>
@@ -10301,7 +10305,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.02</v>
       </c>
@@ -10309,7 +10313,7 @@
         <v>20.29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.2000000000000001E-2</v>
       </c>
@@ -10317,7 +10321,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.8000000000000003E-2</v>
       </c>
@@ -10325,7 +10329,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.10299999999999999</v>
       </c>
@@ -10333,7 +10337,7 @@
         <v>6.98</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.2</v>
       </c>
@@ -10355,20 +10359,20 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>9.859999999999999E-4</v>
       </c>
@@ -10376,7 +10380,7 @@
         <v>45.92</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.7570000000000001E-3</v>
       </c>
@@ -10384,7 +10388,7 @@
         <v>40.9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10392,7 +10396,7 @@
         <v>36.270000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10400,7 +10404,7 @@
         <v>31.77</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.01</v>
       </c>
@@ -10408,7 +10412,7 @@
         <v>25.81</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.02</v>
       </c>
@@ -10416,7 +10420,7 @@
         <v>19.87</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.2000000000000001E-2</v>
       </c>
@@ -10424,7 +10428,7 @@
         <v>15.87</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.8000000000000003E-2</v>
       </c>
@@ -10432,7 +10436,7 @@
         <v>10.91</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.10299999999999999</v>
       </c>
@@ -10440,7 +10444,7 @@
         <v>6.64</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.2</v>
       </c>
@@ -10462,20 +10466,20 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>9.859999999999999E-4</v>
       </c>
@@ -10483,7 +10487,7 @@
         <v>45.99</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.7570000000000001E-3</v>
       </c>
@@ -10491,7 +10495,7 @@
         <v>41.09</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10499,7 +10503,7 @@
         <v>36.47</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10507,7 +10511,7 @@
         <v>32.08</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.01</v>
       </c>
@@ -10515,7 +10519,7 @@
         <v>26.02</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.02</v>
       </c>
@@ -10523,7 +10527,7 @@
         <v>20.07</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.2000000000000001E-2</v>
       </c>
@@ -10531,7 +10535,7 @@
         <v>16.09</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.8000000000000003E-2</v>
       </c>
@@ -10539,7 +10543,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.10299999999999999</v>
       </c>
@@ -10547,7 +10551,7 @@
         <v>6.81</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.2</v>
       </c>
@@ -10569,20 +10573,20 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>9.859999999999999E-4</v>
       </c>
@@ -10590,7 +10594,7 @@
         <v>45.49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.7570000000000001E-3</v>
       </c>
@@ -10598,7 +10602,7 @@
         <v>40.549999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -10606,7 +10610,7 @@
         <v>35.76</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -10614,7 +10618,7 @@
         <v>31.35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.01</v>
       </c>
@@ -10622,7 +10626,7 @@
         <v>25.34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.02</v>
       </c>
@@ -10630,7 +10634,7 @@
         <v>19.45</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.2000000000000001E-2</v>
       </c>
@@ -10638,7 +10642,7 @@
         <v>15.49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5.8000000000000003E-2</v>
       </c>
@@ -10646,7 +10650,7 @@
         <v>10.53</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.10299999999999999</v>
       </c>
@@ -10654,7 +10658,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.2</v>
       </c>

</xml_diff>